<commit_message>
some info fixed in morphological_characterization.xlsx
</commit_message>
<xml_diff>
--- a/source_data/morphological_characterization.xlsx
+++ b/source_data/morphological_characterization.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="1066">
   <si>
     <t xml:space="preserve">Especie</t>
   </si>
@@ -3509,6 +3509,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -14334,6 +14335,9 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="C212" s="0" t="s">
         <v>527</v>
       </c>
@@ -14914,7 +14918,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A212 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17256,7 +17260,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -17272,7 +17276,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A212 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19657,7 +19661,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -19673,7 +19677,7 @@
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="A212 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22669,7 +22673,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -22685,7 +22689,7 @@
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="A212 I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23978,7 +23982,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
allele freqs calculation implemented
</commit_message>
<xml_diff>
--- a/source_data/morphological_characterization.xlsx
+++ b/source_data/morphological_characterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pimpi ECU y PER" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="1070">
   <si>
     <t xml:space="preserve">Especie</t>
   </si>
@@ -2012,9 +2012,21 @@
     <t xml:space="preserve">LA2182</t>
   </si>
   <si>
+    <t xml:space="preserve">055551S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0783946W</t>
+  </si>
+  <si>
     <t xml:space="preserve">LA2188</t>
   </si>
   <si>
+    <t xml:space="preserve">0559--S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07811--W</t>
+  </si>
+  <si>
     <t xml:space="preserve">PE-73</t>
   </si>
   <si>
@@ -2069,6 +2081,9 @@
     <t xml:space="preserve">T-46</t>
   </si>
   <si>
+    <t xml:space="preserve">posición pétalos 1 muy atrás; 2 entre 1 y 3; 3 medio; 4 no</t>
+  </si>
+  <si>
     <t xml:space="preserve">intermedias</t>
   </si>
   <si>
@@ -2565,9 +2580,6 @@
   </si>
   <si>
     <t xml:space="preserve">07959--W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 y 5</t>
   </si>
   <si>
     <t xml:space="preserve">L00712</t>
@@ -3611,12 +3623,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -3628,8 +3640,8 @@
   </sheetPr>
   <dimension ref="A1:W225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A212" activeCellId="0" sqref="A212"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14447,6 +14459,12 @@
       <c r="E214" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G214" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="H214" s="0" t="s">
+        <v>572</v>
+      </c>
       <c r="L214" s="0" t="n">
         <v>2</v>
       </c>
@@ -14468,8 +14486,8 @@
       <c r="R214" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S214" s="0" t="s">
-        <v>161</v>
+      <c r="S214" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="T214" s="0" t="n">
         <v>1</v>
@@ -14489,10 +14507,16 @@
         <v>564</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E215" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G215" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="H215" s="0" t="s">
+        <v>575</v>
       </c>
       <c r="J215" s="0" t="n">
         <v>1</v>
@@ -14542,7 +14566,7 @@
         <v>503</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="E216" s="0" t="n">
         <v>2</v>
@@ -14589,7 +14613,7 @@
         <v>503</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="E217" s="0" t="n">
         <v>2</v>
@@ -14624,13 +14648,13 @@
         <v>209</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="G218" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="H218" s="0" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="R218" s="0" t="n">
         <v>1</v>
@@ -14653,13 +14677,13 @@
         <v>209</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="G219" s="0" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="H219" s="0" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="R219" s="0" t="n">
         <v>1</v>
@@ -14682,13 +14706,13 @@
         <v>209</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="G220" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="H220" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="R220" s="0" t="n">
         <v>1</v>
@@ -14711,7 +14735,7 @@
         <v>61</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="R221" s="0" t="n">
         <v>1</v>
@@ -14737,7 +14761,7 @@
         <v>61</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="K222" s="0" t="n">
         <v>1</v>
@@ -14766,7 +14790,7 @@
         <v>209</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="E223" s="0" t="n">
         <v>1</v>
@@ -14808,7 +14832,7 @@
         <v>1</v>
       </c>
       <c r="W223" s="0" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14819,7 +14843,7 @@
         <v>209</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="E224" s="0" t="n">
         <v>1</v>
@@ -14866,10 +14890,10 @@
         <v>23</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="J225" s="0" t="n">
         <v>1</v>
@@ -14918,7 +14942,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A212 C1"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14926,7 +14950,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14967,7 +14991,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>594</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
@@ -14999,13 +15023,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -15014,10 +15038,10 @@
         <v>5895</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>3</v>
@@ -15061,13 +15085,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -15076,10 +15100,10 @@
         <v>5912</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>3</v>
@@ -15118,18 +15142,18 @@
         <v>4</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -15138,10 +15162,10 @@
         <v>6225</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>3</v>
@@ -15185,10 +15209,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -15197,10 +15221,10 @@
         <v>6229</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>2</v>
@@ -15244,10 +15268,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
@@ -15256,10 +15280,10 @@
         <v>6230</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>3</v>
@@ -15303,10 +15327,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
@@ -15315,10 +15339,10 @@
         <v>6231</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>2</v>
@@ -15356,10 +15380,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
@@ -15368,10 +15392,10 @@
         <v>6232</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>2</v>
@@ -15388,10 +15412,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
@@ -15400,10 +15424,10 @@
         <v>6234</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>3</v>
@@ -15447,10 +15471,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
@@ -15459,10 +15483,10 @@
         <v>6235</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>3</v>
@@ -15512,7 +15536,7 @@
         <v>256</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
@@ -15521,10 +15545,10 @@
         <v>6753</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>3</v>
@@ -15566,7 +15590,7 @@
         <v>4</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15577,7 +15601,7 @@
         <v>256</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
@@ -15586,10 +15610,10 @@
         <v>6767</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>3</v>
@@ -15636,7 +15660,7 @@
         <v>256</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
@@ -15645,10 +15669,10 @@
         <v>6768</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>3</v>
@@ -15698,7 +15722,7 @@
         <v>256</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -15707,10 +15731,10 @@
         <v>6775</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>3</v>
@@ -15752,7 +15776,7 @@
         <v>1</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15763,7 +15787,7 @@
         <v>256</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
@@ -15772,10 +15796,10 @@
         <v>6777</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>3</v>
@@ -15825,7 +15849,7 @@
         <v>256</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -15834,10 +15858,10 @@
         <v>6779</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>3</v>
@@ -15887,7 +15911,7 @@
         <v>256</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -15896,10 +15920,10 @@
         <v>6792</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>3</v>
@@ -15949,7 +15973,7 @@
         <v>256</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -15958,10 +15982,10 @@
         <v>6806</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>1</v>
@@ -16008,10 +16032,10 @@
         <v>255</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -16020,10 +16044,10 @@
         <v>6825</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>3</v>
@@ -16065,7 +16089,7 @@
         <v>4</v>
       </c>
       <c r="W19" s="0" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16073,10 +16097,10 @@
         <v>255</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -16085,10 +16109,10 @@
         <v>6828</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>2</v>
@@ -16130,15 +16154,15 @@
         <v>3</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -16147,10 +16171,10 @@
         <v>6852</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>2</v>
@@ -16197,10 +16221,10 @@
         <v>255</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
@@ -16209,10 +16233,10 @@
         <v>6859</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>1</v>
@@ -16256,10 +16280,10 @@
         <v>255</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
@@ -16268,10 +16292,10 @@
         <v>6865</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>2</v>
@@ -16306,10 +16330,10 @@
         <v>255</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
@@ -16318,10 +16342,10 @@
         <v>6867</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>2</v>
@@ -16362,13 +16386,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
@@ -16377,10 +16401,10 @@
         <v>6881</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>3</v>
@@ -16427,13 +16451,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>
@@ -16442,10 +16466,10 @@
         <v>6896</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>3</v>
@@ -16486,10 +16510,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>1</v>
@@ -16498,10 +16522,10 @@
         <v>6899</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>2</v>
@@ -16542,10 +16566,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
@@ -16554,10 +16578,10 @@
         <v>6901</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>2</v>
@@ -16601,10 +16625,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
@@ -16613,10 +16637,10 @@
         <v>6904</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>3</v>
@@ -16660,13 +16684,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>1</v>
@@ -16675,10 +16699,10 @@
         <v>6906</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>3</v>
@@ -16725,10 +16749,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
@@ -16737,10 +16761,10 @@
         <v>6907</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="L31" s="0" t="n">
         <v>1</v>
@@ -16778,13 +16802,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
@@ -16793,10 +16817,10 @@
         <v>6910</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>680</v>
+        <v>685</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>2</v>
@@ -16837,10 +16861,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
@@ -16849,10 +16873,10 @@
         <v>6927</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>3</v>
@@ -16896,13 +16920,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
@@ -16911,10 +16935,10 @@
         <v>6931</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>687</v>
+        <v>692</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>3</v>
@@ -16961,13 +16985,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
@@ -16976,10 +17000,10 @@
         <v>6934</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>690</v>
+        <v>695</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>3</v>
@@ -17026,10 +17050,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>691</v>
+        <v>696</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
@@ -17038,10 +17062,10 @@
         <v>7015</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>3</v>
@@ -17085,10 +17109,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>691</v>
+        <v>696</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
@@ -17097,10 +17121,10 @@
         <v>7017</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>3</v>
@@ -17144,13 +17168,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1</v>
@@ -17159,10 +17183,10 @@
         <v>7023</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>2</v>
@@ -17206,16 +17230,16 @@
         <v>439</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>12639</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>702</v>
+        <v>707</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>3</v>
@@ -17276,7 +17300,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A212 C1"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17284,7 +17308,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17325,7 +17349,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>594</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
@@ -17357,10 +17381,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -17369,10 +17393,10 @@
         <v>7981</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>3</v>
@@ -17410,19 +17434,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>707</v>
+        <v>712</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>7982</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>3</v>
@@ -17463,10 +17487,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>709</v>
+        <v>714</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -17475,10 +17499,10 @@
         <v>7989</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>710</v>
+        <v>715</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>3</v>
@@ -17522,10 +17546,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -17575,7 +17599,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>508</v>
@@ -17631,10 +17655,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>714</v>
+        <v>719</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
@@ -17643,10 +17667,10 @@
         <v>8036</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>3</v>
@@ -17687,10 +17711,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
@@ -17699,10 +17723,10 @@
         <v>8037</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>3</v>
@@ -17746,10 +17770,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>718</v>
+        <v>723</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
@@ -17758,10 +17782,10 @@
         <v>8041</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>3</v>
@@ -17805,10 +17829,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>719</v>
+        <v>724</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
@@ -17817,10 +17841,10 @@
         <v>8042</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>3</v>
@@ -17864,36 +17888,36 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>714</v>
+        <v>719</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>8044</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>8060</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>3</v>
@@ -17937,10 +17961,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
@@ -17949,10 +17973,10 @@
         <v>8065</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>3</v>
@@ -17999,16 +18023,16 @@
         <v>193</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>8069</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>2</v>
@@ -18052,10 +18076,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
@@ -18064,10 +18088,10 @@
         <v>8077</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>3</v>
@@ -18111,10 +18135,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -18123,10 +18147,10 @@
         <v>8095</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>3</v>
@@ -18170,10 +18194,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -18182,18 +18206,18 @@
         <v>8096</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -18202,10 +18226,10 @@
         <v>8098</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>3</v>
@@ -18252,7 +18276,7 @@
         <v>564</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -18261,10 +18285,10 @@
         <v>8100</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>3</v>
@@ -18308,10 +18332,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>746</v>
+        <v>751</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -18320,10 +18344,10 @@
         <v>8106</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>747</v>
+        <v>752</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>748</v>
+        <v>753</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>3</v>
@@ -18367,10 +18391,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -18379,10 +18403,10 @@
         <v>8108</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>3</v>
@@ -18426,19 +18450,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>8109</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>3</v>
@@ -18482,10 +18506,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
@@ -18494,10 +18518,10 @@
         <v>8189</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>3</v>
@@ -18508,8 +18532,8 @@
       <c r="L23" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="M23" s="0" t="s">
-        <v>756</v>
+      <c r="M23" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="P23" s="0" t="n">
         <v>2</v>
@@ -18535,10 +18559,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
@@ -18547,10 +18571,10 @@
         <v>12625</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>3</v>
@@ -18561,8 +18585,8 @@
       <c r="L24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="M24" s="0" t="s">
-        <v>756</v>
+      <c r="M24" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>2</v>
@@ -18594,10 +18618,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
@@ -18606,10 +18630,10 @@
         <v>12640</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>3</v>
@@ -18653,10 +18677,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>
@@ -18665,10 +18689,10 @@
         <v>13156</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>3</v>
@@ -18712,10 +18736,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>1</v>
@@ -18724,10 +18748,10 @@
         <v>13161</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>2</v>
@@ -18768,19 +18792,19 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>13163</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>1</v>
@@ -18821,10 +18845,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
@@ -18833,10 +18857,10 @@
         <v>13945</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>3</v>
@@ -18877,19 +18901,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>13946</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>3</v>
@@ -18933,10 +18957,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
@@ -18944,10 +18968,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
@@ -18955,22 +18979,22 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>3</v>
@@ -19014,22 +19038,22 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>3</v>
@@ -19070,22 +19094,22 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>3</v>
@@ -19129,22 +19153,22 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>3</v>
@@ -19188,22 +19212,22 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>3</v>
@@ -19247,22 +19271,22 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>3</v>
@@ -19306,22 +19330,22 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>3</v>
@@ -19365,22 +19389,22 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>3</v>
@@ -19424,22 +19448,22 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>3</v>
@@ -19483,22 +19507,22 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>3</v>
@@ -19542,22 +19566,22 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>3</v>
@@ -19601,22 +19625,22 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>3</v>
@@ -19677,7 +19701,7 @@
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="A212 E5"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19687,7 +19711,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19725,7 +19749,7 @@
         <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>13</v>
+        <v>594</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>14</v>
@@ -19758,25 +19782,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>3</v>
@@ -19821,25 +19845,25 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>3</v>
@@ -19884,25 +19908,25 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>3</v>
@@ -19947,25 +19971,25 @@
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>3</v>
@@ -20009,25 +20033,25 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>3</v>
@@ -20066,25 +20090,25 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>3</v>
@@ -20126,25 +20150,25 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>3</v>
@@ -20183,25 +20207,25 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>3</v>
@@ -20243,25 +20267,25 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>3</v>
@@ -20306,25 +20330,25 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>3</v>
@@ -20369,25 +20393,25 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>3</v>
@@ -20429,22 +20453,22 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>3</v>
@@ -20486,22 +20510,22 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>880</v>
+        <v>884</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>3</v>
@@ -20546,22 +20570,22 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>3</v>
@@ -20603,25 +20627,25 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>888</v>
+        <v>892</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>891</v>
+        <v>895</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>3</v>
@@ -20666,25 +20690,25 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>892</v>
+        <v>896</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>2</v>
@@ -20728,25 +20752,25 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>896</v>
+        <v>900</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>2</v>
@@ -20793,43 +20817,43 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="V19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>903</v>
+        <v>907</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>3</v>
@@ -20874,25 +20898,25 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>2</v>
@@ -20937,25 +20961,25 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>3</v>
@@ -20997,30 +21021,30 @@
         <v>2</v>
       </c>
       <c r="V22" s="3" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>3</v>
@@ -21065,22 +21089,22 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>3</v>
@@ -21127,22 +21151,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>927</v>
+        <v>931</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>3</v>
@@ -21187,22 +21211,22 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>931</v>
+        <v>935</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>3</v>
@@ -21247,22 +21271,22 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>3</v>
@@ -21307,22 +21331,22 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>2</v>
@@ -21355,22 +21379,22 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>3</v>
@@ -21415,22 +21439,22 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>953</v>
+        <v>957</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>3</v>
@@ -21475,16 +21499,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>3</v>
@@ -21526,16 +21550,16 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>3</v>
@@ -21577,22 +21601,22 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>3</v>
@@ -21637,22 +21661,22 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>961</v>
+        <v>965</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>3</v>
@@ -21697,25 +21721,25 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>963</v>
+        <v>967</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>3</v>
@@ -21754,22 +21778,22 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>966</v>
+        <v>970</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>3</v>
@@ -21814,22 +21838,22 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>967</v>
+        <v>971</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>968</v>
+        <v>972</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>2</v>
@@ -21874,22 +21898,22 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>969</v>
+        <v>973</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>970</v>
+        <v>974</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>971</v>
+        <v>975</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>3</v>
@@ -21934,22 +21958,22 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>3</v>
@@ -21991,25 +22015,25 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>3</v>
@@ -22054,22 +22078,22 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>981</v>
+        <v>985</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>982</v>
+        <v>986</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>3</v>
@@ -22114,13 +22138,13 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>983</v>
+        <v>987</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>984</v>
+        <v>988</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>3</v>
@@ -22165,22 +22189,22 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>985</v>
+        <v>989</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G43" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="H43" s="0" t="s">
         <v>833</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>829</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>3</v>
@@ -22222,22 +22246,22 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>986</v>
+        <v>990</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>987</v>
+        <v>991</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>3</v>
@@ -22279,22 +22303,22 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>989</v>
+        <v>993</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>3</v>
@@ -22336,27 +22360,27 @@
         <v>2</v>
       </c>
       <c r="V45" s="3" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>3</v>
@@ -22398,18 +22422,18 @@
         <v>4</v>
       </c>
       <c r="V46" s="3" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>1</v>
@@ -22454,30 +22478,30 @@
         <v>4</v>
       </c>
       <c r="V47" s="3" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c r="V48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>993</v>
+        <v>997</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>2</v>
@@ -22519,10 +22543,10 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>1</v>
@@ -22570,10 +22594,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>996</v>
+        <v>1000</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>1</v>
@@ -22621,10 +22645,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>997</v>
+        <v>1001</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>1</v>
@@ -22688,8 +22712,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="A212 I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22697,7 +22721,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -22735,7 +22759,7 @@
         <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>13</v>
+        <v>594</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>14</v>
@@ -22768,25 +22792,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>999</v>
+        <v>1003</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1000</v>
+        <v>1004</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>3</v>
@@ -22830,25 +22854,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>3</v>
@@ -22892,25 +22916,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>3</v>
@@ -22948,22 +22972,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>3</v>
@@ -23007,25 +23031,25 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1015</v>
+        <v>1019</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>3</v>
@@ -23036,8 +23060,8 @@
       <c r="K6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="0" t="s">
-        <v>396</v>
+      <c r="L6" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>2</v>
@@ -23069,25 +23093,25 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>3</v>
@@ -23098,8 +23122,8 @@
       <c r="K7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="0" t="s">
-        <v>396</v>
+      <c r="L7" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>2</v>
@@ -23131,25 +23155,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1021</v>
+        <v>1025</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>3</v>
@@ -23193,25 +23217,25 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>1024</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>1016</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>1020</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>3</v>
@@ -23255,22 +23279,22 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>3</v>
@@ -23314,25 +23338,25 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>3</v>
@@ -23376,22 +23400,22 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>3</v>
@@ -23435,22 +23459,22 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1036</v>
+        <v>1040</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>3</v>
@@ -23494,25 +23518,25 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>3</v>
@@ -23556,25 +23580,25 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>3</v>
@@ -23618,25 +23642,25 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>3</v>
@@ -23680,22 +23704,22 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>3</v>
@@ -23739,25 +23763,25 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>1053</v>
+        <v>1057</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>3</v>
@@ -23801,25 +23825,25 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1054</v>
+        <v>1058</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>3</v>
@@ -23860,25 +23884,25 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1059</v>
+        <v>1063</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>1061</v>
+        <v>1065</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>3</v>
@@ -23922,25 +23946,25 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>3</v>

</xml_diff>